<commit_message>
fixed a couple of warnings
</commit_message>
<xml_diff>
--- a/TESTING.xlsx
+++ b/TESTING.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="49">
   <si>
     <t>toolset=clang cxxstd=14</t>
   </si>
@@ -134,13 +134,43 @@
     <t>toolset cxxstd=11 -q</t>
   </si>
   <si>
-    <t>errors</t>
-  </si>
-  <si>
     <t>cmd</t>
   </si>
   <si>
-    <t>rm -f ../../../bin.v2/project-cache.jam ; ../../../b2 -q toolset=msvc cxxstd=11 link=shared bc_no=all_yes,yi,pe,xi,po,ex,ck,yi_pe,yi_xi,yi_po,yi_ex,yi_ck,pe_xi,pe_po,pe_ex,pe_ck,xi_po,xi_ex,xi_ck,po_ex,po_ck,ex_ck,yi_pe_xi,yi_pe_po,yi_pe_ex,yi_pe_ck,yi_xi_po,yi_xi_ex,yi_xi_ck,yi_po_ex,yi_po_ck,yi_ex_ck,pe_xi_po,pe_xi_ex,pe_xi_ck,pe_po_ex,pe_po_ck,pe_ex_ck,xi_po_ex,xi_po_ck,xi_ex_ck,po_ex_ck,yi_pe_xi_po,yi_pe_xi_ex,yi_pe_xi_ck,yi_pe_po_ex,yi_pe_po_ck,yi_pe_ex_ck,yi_xi_po_ex,yi_xi_po_ck,yi_xi_ex_ck,yi_po_ex_ck,pe_xi_po_ex,pe_xi_po_ck,pe_xi_ex_ck,pe_po_ex_ck,xi_po_ex_ck,yi_pe_xi_po_ex,yi_pe_xi_po_ck,yi_pe_xi_ex_ck,yi_pe_po_ex_ck,yi_xi_po_ex_ck,pe_xi_po_ex_ck,yi_pe_xi_po_ex_ck &gt;&gt; 00.out ; echo $? ; beep -1</t>
+    <t>msvc,gcc,clang</t>
+  </si>
+  <si>
+    <t>rm -f ../../../bin.v2/project-cache.jam ; ../../../b2 -q toolset=msvc,gcc,clang cxxstd=11 link=shared,static bc_no=all_yes,yi_pe_xi_po_ex_ck &gt; 00.out ; echo $? ; beep -1</t>
+  </si>
+  <si>
+    <t>shared,static</t>
+  </si>
+  <si>
+    <t>all_yes,all_no</t>
+  </si>
+  <si>
+    <t>rm -f ../../../bin.v2/project-cache.jam ; ../../../b2 -q toolset=msvc,gcc,clang cxxstd=11 bc_hdr=only bc_no=all_yes,yi_pe_xi_po_ex_ck &gt; 00.out ; echo $? ; beep -1</t>
+  </si>
+  <si>
+    <t>6.6GB</t>
+  </si>
+  <si>
+    <t>Free disk space w/o bin.v2/lib/contract dir = 84GB</t>
+  </si>
+  <si>
+    <t>errors (smoke)</t>
+  </si>
+  <si>
+    <t>errors (all)</t>
+  </si>
+  <si>
+    <t>rm -f ../../../bin.v2/project-cache.jam ; ../../../b2 -q toolset=msvc cxxstd=11 link=shared bc_no=all_yes,yi,pe,xi,po,ex,ck,yi_pe,yi_xi,yi_po,yi_ex,yi_ck,pe_xi,pe_po,pe_ex,pe_ck,xi_po,xi_ex,xi_ck,po_ex,po_ck,ex_ck,yi_pe_xi,yi_pe_po,yi_pe_ex,yi_pe_ck,yi_xi_po,yi_xi_ex,yi_xi_ck,yi_po_ex,yi_po_ck,yi_ex_ck,pe_xi_po,pe_xi_ex,pe_xi_ck,pe_po_ex,pe_po_ck,pe_ex_ck,xi_po_ex,xi_po_ck,xi_ex_ck,po_ex_ck,yi_pe_xi_po,yi_pe_xi_ex,yi_pe_xi_ck,yi_pe_po_ex,yi_pe_po_ck,yi_pe_ex_ck,yi_xi_po_ex,yi_xi_po_ck,yi_xi_ex_ck,yi_po_ex_ck,pe_xi_po_ex,pe_xi_po_ck,pe_xi_ex_ck,pe_po_ex_ck,xi_po_ex_ck,yi_pe_xi_po_ex,yi_pe_xi_po_ck,yi_pe_xi_ex_ck,yi_pe_po_ex_ck,yi_xi_po_ex_ck,pe_xi_po_ex_ck,yi_pe_xi_po_ex_ck &gt; 00.out ; echo $? ; beep -1</t>
+  </si>
+  <si>
+    <t>cxxstd=14</t>
+  </si>
+  <si>
+    <t>test/…cxx14… (only 1 test?)</t>
   </si>
 </sst>
 </file>
@@ -492,12 +522,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:G47"/>
+  <dimension ref="A2:G60"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <pane ySplit="900" topLeftCell="A13" activePane="bottomLeft"/>
-      <selection activeCell="G15" sqref="G15"/>
-      <selection pane="bottomLeft" activeCell="G48" sqref="G48"/>
+      <pane ySplit="900" topLeftCell="A31" activePane="bottomLeft"/>
+      <selection activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,6 +537,14 @@
     <col min="8" max="16384" width="36.42578125" style="3"/>
   </cols>
   <sheetData>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
     </row>
@@ -598,7 +636,7 @@
         <v>23</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -918,22 +956,116 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>32</v>
+        <v>40</v>
+      </c>
+      <c r="F47" s="3">
+        <v>2</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D48" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F48" s="3">
+        <v>2</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D51" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D52" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C53" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D54" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D55" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C56" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D57" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D58" s="3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
renamed bc_no options to use single letter flags. compiled all test with toolset=msvc,gcc,clang with link=shared,static and bc_hdr=only with bc_no=all_yes and all no combinations check no errors and no warnings
</commit_message>
<xml_diff>
--- a/TESTING.xlsx
+++ b/TESTING.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="56">
   <si>
     <t>toolset=clang cxxstd=14</t>
   </si>
@@ -140,18 +140,12 @@
     <t>msvc,gcc,clang</t>
   </si>
   <si>
-    <t>rm -f ../../../bin.v2/project-cache.jam ; ../../../b2 -q toolset=msvc,gcc,clang cxxstd=11 link=shared,static bc_no=all_yes,yi_pe_xi_po_ex_ck &gt; 00.out ; echo $? ; beep -1</t>
-  </si>
-  <si>
     <t>shared,static</t>
   </si>
   <si>
     <t>all_yes,all_no</t>
   </si>
   <si>
-    <t>rm -f ../../../bin.v2/project-cache.jam ; ../../../b2 -q toolset=msvc,gcc,clang cxxstd=11 bc_hdr=only bc_no=all_yes,yi_pe_xi_po_ex_ck &gt; 00.out ; echo $? ; beep -1</t>
-  </si>
-  <si>
     <t>6.6GB</t>
   </si>
   <si>
@@ -164,13 +158,40 @@
     <t>errors (all)</t>
   </si>
   <si>
-    <t>rm -f ../../../bin.v2/project-cache.jam ; ../../../b2 -q toolset=msvc cxxstd=11 link=shared bc_no=all_yes,yi,pe,xi,po,ex,ck,yi_pe,yi_xi,yi_po,yi_ex,yi_ck,pe_xi,pe_po,pe_ex,pe_ck,xi_po,xi_ex,xi_ck,po_ex,po_ck,ex_ck,yi_pe_xi,yi_pe_po,yi_pe_ex,yi_pe_ck,yi_xi_po,yi_xi_ex,yi_xi_ck,yi_po_ex,yi_po_ck,yi_ex_ck,pe_xi_po,pe_xi_ex,pe_xi_ck,pe_po_ex,pe_po_ck,pe_ex_ck,xi_po_ex,xi_po_ck,xi_ex_ck,po_ex_ck,yi_pe_xi_po,yi_pe_xi_ex,yi_pe_xi_ck,yi_pe_po_ex,yi_pe_po_ck,yi_pe_ex_ck,yi_xi_po_ex,yi_xi_po_ck,yi_xi_ex_ck,yi_po_ex_ck,pe_xi_po_ex,pe_xi_po_ck,pe_xi_ex_ck,pe_po_ex_ck,xi_po_ex_ck,yi_pe_xi_po_ex,yi_pe_xi_po_ck,yi_pe_xi_ex_ck,yi_pe_po_ex_ck,yi_xi_po_ex_ck,pe_xi_po_ex_ck,yi_pe_xi_po_ex_ck &gt; 00.out ; echo $? ; beep -1</t>
-  </si>
-  <si>
     <t>cxxstd=14</t>
   </si>
   <si>
-    <t>test/…cxx14… (only 1 test?)</t>
+    <t>rm -f ../../../bin.v2/project-cache.jam ; ../../../b2 -q toolset=msvc cxxstd=11 link=shared bc_no=all_yes,yi,pe,xi,po,ex,ck,yi_pe,yi_xi,yi_po,yi_ex,yi_ck,pe_xi,pe_po,pe_ex,pe_ck,xi_po,xi_ex,xi_ck,po_ex,po_ck,ex_ck,yi_pe_xi,yi_pe_po,yi_pe_ex,yi_pe_ck,yi_xi_po,yi_xi_ex,yi_xi_ck,yi_po_ex,yi_po_ck,yi_ex_ck,pe_xi_po,pe_xi_ex,pe_xi_ck,pe_po_ex,pe_po_ck,pe_ex_ck,xi_po_ex,xi_po_ck,xi_ex_ck,po_ex_ck,yi_pe_xi_po,yi_pe_xi_ex,yi_pe_xi_ck,yi_pe_po_ex,yi_pe_po_ck,yi_pe_ex_ck,yi_xi_po_ex,yi_xi_po_ck,yi_xi_ex_ck,yi_po_ex_ck,pe_xi_po_ex,pe_xi_po_ck,pe_xi_ex_ck,pe_po_ex_ck,xi_po_ex_ck,yi_pe_xi_po_ex,yi_pe_xi_po_ck,yi_pe_xi_ex_ck,yi_pe_po_ex_ck,yi_xi_po_ex_ck,pe_xi_po_ex_ck,yi_pe_xi_po_ex_ck &gt;&gt; 00.out ; echo $? ; beep -1</t>
+  </si>
+  <si>
+    <t>rm -f ../../../bin.v2/project-cache.jam ; ../../../b2 -q toolset=msvc,gcc,clang cxxstd=11 bc_hdr=only bc_no=all_yes,yi_pe_xi_po_ex_ck &gt;&gt; 00.out ; echo $? ; beep -1</t>
+  </si>
+  <si>
+    <t>rm -f ../../../bin.v2/project-cache.jam ; ../../../b2 -q toolset=msvc,gcc,clang cxxstd=11 link=shared,static bc_no=all_yes,yi_pe_xi_po_ex_ck &gt;&gt; 00.out ; echo $? ; beep -1</t>
+  </si>
+  <si>
+    <t>after msvc shared all = 33GB</t>
+  </si>
+  <si>
+    <t>rm -f ../../../bin.v2/project-cache.jam ; ../../../b2 -q toolset=clang cxxstd=11 link=static bc_no=all_yes,yi,pe,xi,po,ex,ck,yi_pe,yi_xi,yi_po,yi_ex,yi_ck,pe_xi,pe_po,pe_ex,pe_ck,xi_po,xi_ex,xi_ck,po_ex,po_ck,ex_ck,yi_pe_xi,yi_pe_po,yi_pe_ex,yi_pe_ck,yi_xi_po,yi_xi_ex,yi_xi_ck,yi_po_ex,yi_po_ck,yi_ex_ck,pe_xi_po,pe_xi_ex,pe_xi_ck,pe_po_ex,pe_po_ck,pe_ex_ck,xi_po_ex,xi_po_ck,xi_ex_ck,po_ex_ck,yi_pe_xi_po,yi_pe_xi_ex,yi_pe_xi_ck,yi_pe_po_ex,yi_pe_po_ck,yi_pe_ex_ck,yi_xi_po_ex,yi_xi_po_ck,yi_xi_ex_ck,yi_po_ex_ck,pe_xi_po_ex,pe_xi_po_ck,pe_xi_ex_ck,pe_po_ex_ck,xi_po_ex_ck,yi_pe_xi_po_ex,yi_pe_xi_po_ck,yi_pe_xi_ex_ck,yi_pe_po_ex_ck,yi_xi_po_ex_ck,pe_xi_po_ex_ck,yi_pe_xi_po_ex_ck &gt;&gt; 00.out ; echo $? ; beep -1</t>
+  </si>
+  <si>
+    <t>rm -f ../../../bin.v2/project-cache.jam ; ../../../b2 -q toolset=clang cxxstd=11 link=shared bc_no=all_yes,yi,pe,xi,po,ex,ck,yi_pe,yi_xi,yi_po,yi_ex,yi_ck,pe_xi,pe_po,pe_ex,pe_ck,xi_po,xi_ex,xi_ck,po_ex,po_ck,ex_ck,yi_pe_xi,yi_pe_po,yi_pe_ex,yi_pe_ck,yi_xi_po,yi_xi_ex,yi_xi_ck,yi_po_ex,yi_po_ck,yi_ex_ck,pe_xi_po,pe_xi_ex,pe_xi_ck,pe_po_ex,pe_po_ck,pe_ex_ck,xi_po_ex,xi_po_ck,xi_ex_ck,po_ex_ck,yi_pe_xi_po,yi_pe_xi_ex,yi_pe_xi_ck,yi_pe_po_ex,yi_pe_po_ck,yi_pe_ex_ck,yi_xi_po_ex,yi_xi_po_ck,yi_xi_ex_ck,yi_po_ex_ck,pe_xi_po_ex,pe_xi_po_ck,pe_xi_ex_ck,pe_po_ex_ck,xi_po_ex_ck,yi_pe_xi_po_ex,yi_pe_xi_po_ck,yi_pe_xi_ex_ck,yi_pe_po_ex_ck,yi_xi_po_ex_ck,pe_xi_po_ex_ck,yi_pe_xi_po_ex_ck &gt;&gt; 00.out ; echo $? ; beep -1</t>
+  </si>
+  <si>
+    <t>rm -f ../../../bin.v2/project-cache.jam ; ../../../b2 -q toolset=gcc cxxstd=11 link=shared bc_no=all_yes,yi,pe,xi,po,ex,ck,yi_pe,yi_xi,yi_po,yi_ex,yi_ck,pe_xi,pe_po,pe_ex,pe_ck,xi_po,xi_ex,xi_ck,po_ex,po_ck,ex_ck,yi_pe_xi,yi_pe_po,yi_pe_ex,yi_pe_ck,yi_xi_po,yi_xi_ex,yi_xi_ck,yi_po_ex,yi_po_ck,yi_ex_ck,pe_xi_po,pe_xi_ex,pe_xi_ck,pe_po_ex,pe_po_ck,pe_ex_ck,xi_po_ex,xi_po_ck,xi_ex_ck,po_ex_ck,yi_pe_xi_po,yi_pe_xi_ex,yi_pe_xi_ck,yi_pe_po_ex,yi_pe_po_ck,yi_pe_ex_ck,yi_xi_po_ex,yi_xi_po_ck,yi_xi_ex_ck,yi_po_ex_ck,pe_xi_po_ex,pe_xi_po_ck,pe_xi_ex_ck,pe_po_ex_ck,xi_po_ex_ck,yi_pe_xi_po_ex,yi_pe_xi_po_ck,yi_pe_xi_ex_ck,yi_pe_po_ex_ck,yi_xi_po_ex_ck,pe_xi_po_ex_ck,yi_pe_xi_po_ex_ck &gt;&gt; 00.out ; echo $? ; beep -1</t>
+  </si>
+  <si>
+    <t>rm -f ../../../bin.v2/project-cache.jam ; ../../../b2 -q toolset=gcc cxxstd=11 link=static bc_no=all_yes,yi,pe,xi,po,ex,ck,yi_pe,yi_xi,yi_po,yi_ex,yi_ck,pe_xi,pe_po,pe_ex,pe_ck,xi_po,xi_ex,xi_ck,po_ex,po_ck,ex_ck,yi_pe_xi,yi_pe_po,yi_pe_ex,yi_pe_ck,yi_xi_po,yi_xi_ex,yi_xi_ck,yi_po_ex,yi_po_ck,yi_ex_ck,pe_xi_po,pe_xi_ex,pe_xi_ck,pe_po_ex,pe_po_ck,pe_ex_ck,xi_po_ex,xi_po_ck,xi_ex_ck,po_ex_ck,yi_pe_xi_po,yi_pe_xi_ex,yi_pe_xi_ck,yi_pe_po_ex,yi_pe_po_ck,yi_pe_ex_ck,yi_xi_po_ex,yi_xi_po_ck,yi_xi_ex_ck,yi_po_ex_ck,pe_xi_po_ex,pe_xi_po_ck,pe_xi_ex_ck,pe_po_ex_ck,xi_po_ex_ck,yi_pe_xi_po_ex,yi_pe_xi_po_ck,yi_pe_xi_ex_ck,yi_pe_po_ex_ck,yi_xi_po_ex_ck,pe_xi_po_ex_ck,yi_pe_xi_po_ex_ck &gt;&gt; 00.out ; echo $? ; beep -1</t>
+  </si>
+  <si>
+    <t>rm -f ../../../bin.v2/project-cache.jam ; ../../../b2 -q toolset=clang cxxstd=11 bc_hdr=only bc_no=all_yes,y,r,x,s,e,k,yr,yx,ys,ye,yk,rx,rs,re,rk,xs,xe,xk,se,sk,ek,yrx,yrs,yre,yrk,yxs,yxe,yxk,yse,ysk,yek,rxs,rxe,rxk,rse,rsk,rek,xse,xsk,xek,sek,yrxs,yrxe,yrxk,yrse,yrsk,yrek,yxse,yxsk,yxek,ysek,rxse,rxsk,rxek,rsek,xsek,yrxse,yrxsk,yrxek,yrsek,yxsek,rxsek,yrxsek &gt; 00.out ; echo $? ; beep -1</t>
+  </si>
+  <si>
+    <t>test (call_if-equal_to_cxx14)</t>
+  </si>
+  <si>
+    <t>example (features-call_if_cxx14)</t>
   </si>
 </sst>
 </file>
@@ -522,12 +543,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G60"/>
+  <dimension ref="A2:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <pane ySplit="900" topLeftCell="A31" activePane="bottomLeft"/>
+      <pane ySplit="900" activePane="bottomLeft"/>
       <selection activeCell="E16" sqref="E16"/>
-      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -539,10 +560,13 @@
   <sheetData>
     <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -956,7 +980,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B47" s="3" t="s">
         <v>6</v>
@@ -965,16 +989,16 @@
         <v>37</v>
       </c>
       <c r="D47" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="F47" s="3">
         <v>2</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -985,12 +1009,12 @@
         <v>2</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B50" s="3" t="s">
         <v>6</v>
@@ -1004,19 +1028,28 @@
       <c r="E50" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="F50" s="3">
+        <v>2</v>
+      </c>
       <c r="G50" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D51" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="F51" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D52" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="F52" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C53" s="3" t="s">
@@ -1028,16 +1061,31 @@
       <c r="E53" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="F53" s="3">
+        <v>2</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D54" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="F54" s="3">
+        <v>2</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D55" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="F55" s="3">
+        <v>2</v>
+      </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C56" s="3" t="s">
@@ -1049,23 +1097,86 @@
       <c r="E56" s="3" t="s">
         <v>32</v>
       </c>
+      <c r="F56" s="3">
+        <v>2</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D57" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="F57" s="3">
+        <v>2</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D58" s="3" t="s">
         <v>24</v>
       </c>
+      <c r="F58" s="3">
+        <v>2</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B60" s="3" t="s">
-        <v>48</v>
+        <v>54</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D60" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E60" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F60" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D61" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F61" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B62" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D62" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F62" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D63" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F63" s="3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
building all combinations for examples
</commit_message>
<xml_diff>
--- a/TESTING.xlsx
+++ b/TESTING.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="60">
   <si>
     <t>toolset=clang cxxstd=14</t>
   </si>
@@ -192,6 +192,18 @@
   </si>
   <si>
     <t>example (features-call_if_cxx14)</t>
+  </si>
+  <si>
+    <t>example</t>
+  </si>
+  <si>
+    <t>msvc,clang</t>
+  </si>
+  <si>
+    <t>all example errors &amp; warnings</t>
+  </si>
+  <si>
+    <t>msvc,clang,gcc</t>
   </si>
 </sst>
 </file>
@@ -543,12 +555,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G63"/>
+  <dimension ref="A2:G66"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <pane ySplit="900" activePane="bottomLeft"/>
+      <pane ySplit="900" topLeftCell="A43" activePane="bottomLeft"/>
       <selection activeCell="E16" sqref="E16"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1179,6 +1191,34 @@
         <v>2</v>
       </c>
     </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D66" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
compiled all examples with all combinations. also compiled all tests and examples with c++03
</commit_message>
<xml_diff>
--- a/TESTING.xlsx
+++ b/TESTING.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="59">
   <si>
     <t>toolset=clang cxxstd=14</t>
   </si>
@@ -195,9 +195,6 @@
   </si>
   <si>
     <t>example</t>
-  </si>
-  <si>
-    <t>msvc,clang</t>
   </si>
   <si>
     <t>all example errors &amp; warnings</t>
@@ -560,7 +557,7 @@
     <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
       <pane ySplit="900" topLeftCell="A43" activePane="bottomLeft"/>
       <selection activeCell="E16" sqref="E16"/>
-      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
+      <selection pane="bottomLeft" activeCell="F67" sqref="F67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1193,7 +1190,7 @@
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B65" s="3" t="s">
         <v>56</v>
@@ -1208,7 +1205,7 @@
         <v>32</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1216,7 +1213,7 @@
         <v>24</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>